<commit_message>
Acoes internacionais e Renda fixa
Correção do erro onde a aba de ações internacionais e renda fixa da planilha eram exportadas com os valores zerados.
</commit_message>
<xml_diff>
--- a/cotacoes_bolsa.xlsx
+++ b/cotacoes_bolsa.xlsx
@@ -473,17 +473,17 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>11.77999973297119</v>
+        <v>12.30646991729736</v>
       </c>
       <c r="C2" t="n">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>636.1199855804443</v>
+        <v>12.30646991729736</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>24/11/2025 08:37:50</t>
+          <t>01/12/2025 09:04:44</t>
         </is>
       </c>
     </row>
@@ -494,17 +494,17 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>22</v>
+        <v>22.46999931335449</v>
       </c>
       <c r="C3" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>660</v>
+        <v>22.46999931335449</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>24/11/2025 08:37:51</t>
+          <t>01/12/2025 09:04:44</t>
         </is>
       </c>
     </row>
@@ -515,17 +515,17 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>13.61999988555908</v>
+        <v>13.85999965667725</v>
       </c>
       <c r="C4" t="n">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>558.4199953079224</v>
+        <v>13.85999965667725</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>24/11/2025 08:37:51</t>
+          <t>01/12/2025 09:04:44</t>
         </is>
       </c>
     </row>
@@ -536,17 +536,17 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>34.47999954223633</v>
+        <v>35.43000030517578</v>
       </c>
       <c r="C5" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>620.6399917602539</v>
+        <v>35.43000030517578</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>24/11/2025 08:37:51</t>
+          <t>01/12/2025 09:04:45</t>
         </is>
       </c>
     </row>
@@ -557,17 +557,17 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>65.16000366210938</v>
+        <v>67.40000152587891</v>
       </c>
       <c r="C6" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>586.4400329589844</v>
+        <v>67.40000152587891</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>24/11/2025 08:37:51</t>
+          <t>01/12/2025 09:04:45</t>
         </is>
       </c>
     </row>
@@ -578,17 +578,17 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>18.29000091552734</v>
+        <v>19.43000030517578</v>
       </c>
       <c r="C7" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>640.150032043457</v>
+        <v>19.43000030517578</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>24/11/2025 08:37:51</t>
+          <t>01/12/2025 09:04:45</t>
         </is>
       </c>
     </row>
@@ -599,17 +599,17 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>11.01000022888184</v>
+        <v>11.5</v>
       </c>
       <c r="C8" t="n">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>583.5300121307373</v>
+        <v>11.5</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>24/11/2025 08:37:51</t>
+          <t>01/12/2025 09:04:45</t>
         </is>
       </c>
     </row>
@@ -620,17 +620,17 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>42.63999938964844</v>
+        <v>30.63999938964844</v>
       </c>
       <c r="C9" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>596.9599914550781</v>
+        <v>30.63999938964844</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>24/11/2025 08:37:51</t>
+          <t>01/12/2025 09:04:45</t>
         </is>
       </c>
     </row>
@@ -641,17 +641,17 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>37.88999938964844</v>
+        <v>41.63000106811523</v>
       </c>
       <c r="C10" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>947.2499847412109</v>
+        <v>41.63000106811523</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>24/11/2025 08:37:52</t>
+          <t>01/12/2025 09:04:45</t>
         </is>
       </c>
     </row>
@@ -662,17 +662,17 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>6.75</v>
+        <v>7.360000133514404</v>
       </c>
       <c r="C11" t="n">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>540</v>
+        <v>7.360000133514404</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>24/11/2025 08:37:52</t>
+          <t>01/12/2025 09:04:46</t>
         </is>
       </c>
     </row>
@@ -698,7 +698,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Ação</t>
+          <t>Ação:</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -729,17 +729,17 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>5.399300098419189</v>
+        <v>5.334199905395508</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0</v>
+        <v>5.334199905395508</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>24/11/2025 08:38:21</t>
+          <t>01/12/2025 09:04:50</t>
         </is>
       </c>
     </row>
@@ -750,17 +750,17 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>5.399300098419189</v>
+        <v>5.334199905395508</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0</v>
+        <v>5.334199905395508</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>24/11/2025 08:38:21</t>
+          <t>01/12/2025 09:04:50</t>
         </is>
       </c>
     </row>
@@ -771,17 +771,17 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>5.399300098419189</v>
+        <v>5.334199905395508</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0</v>
+        <v>5.334199905395508</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>24/11/2025 08:38:21</t>
+          <t>01/12/2025 09:04:50</t>
         </is>
       </c>
     </row>
@@ -792,17 +792,17 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>5.399300098419189</v>
+        <v>5.334199905395508</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>0</v>
+        <v>5.334199905395508</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>24/11/2025 08:38:21</t>
+          <t>01/12/2025 09:04:50</t>
         </is>
       </c>
     </row>
@@ -859,17 +859,17 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>150</v>
+        <v>151.0399932861328</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>900</v>
+        <v>151.0399932861328</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>24/11/2025 08:38:40</t>
+          <t>01/12/2025 09:04:58</t>
         </is>
       </c>
     </row>
@@ -880,17 +880,17 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>86.98999786376953</v>
+        <v>87.25</v>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>695.9199829101562</v>
+        <v>87.25</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>24/11/2025 08:38:40</t>
+          <t>01/12/2025 09:04:58</t>
         </is>
       </c>
     </row>
@@ -901,17 +901,17 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>9.909999847412109</v>
+        <v>9.920000076293945</v>
       </c>
       <c r="C4" t="n">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>693.6999893188477</v>
+        <v>9.920000076293945</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>24/11/2025 08:38:40</t>
+          <t>01/12/2025 09:04:58</t>
         </is>
       </c>
     </row>
@@ -922,17 +922,17 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>82.13999938964844</v>
+        <v>83.04000091552734</v>
       </c>
       <c r="C5" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>657.1199951171875</v>
+        <v>83.04000091552734</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>24/11/2025 08:38:40</t>
+          <t>01/12/2025 09:04:59</t>
         </is>
       </c>
     </row>
@@ -943,17 +943,17 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>109.5999984741211</v>
+        <v>109.5800018310547</v>
       </c>
       <c r="C6" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>767.1999893188477</v>
+        <v>109.5800018310547</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>24/11/2025 08:38:40</t>
+          <t>01/12/2025 09:04:59</t>
         </is>
       </c>
     </row>
@@ -964,17 +964,17 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>78.08999633789062</v>
+        <v>79.23000335693359</v>
       </c>
       <c r="C7" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>624.719970703125</v>
+        <v>79.23000335693359</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>24/11/2025 08:38:41</t>
+          <t>01/12/2025 09:04:59</t>
         </is>
       </c>
     </row>
@@ -985,17 +985,17 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>79.33999633789062</v>
+        <v>79.87000274658203</v>
       </c>
       <c r="C8" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>634.719970703125</v>
+        <v>79.87000274658203</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>24/11/2025 08:38:41</t>
+          <t>01/12/2025 09:04:59</t>
         </is>
       </c>
     </row>
@@ -1006,17 +1006,17 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>88</v>
+        <v>88.27999877929688</v>
       </c>
       <c r="C9" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>704</v>
+        <v>88.27999877929688</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>24/11/2025 08:38:41</t>
+          <t>01/12/2025 09:04:59</t>
         </is>
       </c>
     </row>
@@ -1030,14 +1030,14 @@
         <v>64.48999786376953</v>
       </c>
       <c r="C10" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>709.3899765014648</v>
+        <v>64.48999786376953</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>24/11/2025 08:38:41</t>
+          <t>01/12/2025 09:04:59</t>
         </is>
       </c>
     </row>
@@ -1051,14 +1051,14 @@
         <v>8.380000114440918</v>
       </c>
       <c r="C11" t="n">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>586.6000080108643</v>
+        <v>8.380000114440918</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>24/11/2025 08:38:41</t>
+          <t>01/12/2025 09:05:00</t>
         </is>
       </c>
     </row>
@@ -1069,17 +1069,17 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="C12" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>500</v>
+        <v>5.25</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>24/11/2025 08:38:41</t>
+          <t>01/12/2025 09:05:00</t>
         </is>
       </c>
     </row>
@@ -1090,17 +1090,17 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>9.569999694824219</v>
+        <v>9.630000114440918</v>
       </c>
       <c r="C13" t="n">
-        <v>68</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>650.7599792480469</v>
+        <v>9.630000114440918</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>24/11/2025 08:38:42</t>
+          <t>01/12/2025 09:05:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1126,15 +1126,25 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Categoria</t>
+          <t>Ação</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Total Investido (R$)</t>
+          <t>Valor em USD</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Cotação Dolar</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Valor em Reais</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Atualizado em</t>
         </is>
@@ -1146,12 +1156,12 @@
           <t>Renda Fixa</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>24/11/2025 08:38:57</t>
+      <c r="D2" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>01/12/2025 09:05:04</t>
         </is>
       </c>
     </row>

</xml_diff>